<commit_message>
Merged code of Eng
</commit_message>
<xml_diff>
--- a/TestData/T2189_PortfolioValuationCreation.xlsx
+++ b/TestData/T2189_PortfolioValuationCreation.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SGoyal0427\source\repos\SalesForce_Project\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sgoyal0427\source\repos\SalesForce_Project\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="7416" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="2370" windowHeight="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="2" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="71">
   <si>
     <t>StdUser</t>
   </si>
@@ -244,6 +244,9 @@
   </si>
   <si>
     <t>Chris Lord</t>
+  </si>
+  <si>
+    <t>10000.0</t>
   </si>
 </sst>
 </file>
@@ -582,13 +585,13 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
     <col min="2" max="2" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -596,7 +599,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>68</v>
       </c>
@@ -613,24 +616,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.5546875" customWidth="1"/>
-    <col min="8" max="8" width="13.88671875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="28.44140625" customWidth="1"/>
-    <col min="13" max="13" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.5703125" customWidth="1"/>
+    <col min="8" max="8" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="28.42578125" customWidth="1"/>
+    <col min="13" max="13" width="9.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>22</v>
       </c>
@@ -671,7 +674,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>23</v>
       </c>
@@ -722,18 +725,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB2"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="X7" sqref="X7"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="AA3" sqref="AA3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="26.33203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="26.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="26.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>26</v>
       </c>
@@ -819,7 +822,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>67</v>
       </c>
@@ -899,7 +902,7 @@
         <v>25</v>
       </c>
       <c r="AA2" s="4" t="s">
-        <v>59</v>
+        <v>70</v>
       </c>
       <c r="AB2" s="4" t="s">
         <v>59</v>

</xml_diff>